<commit_message>
Exploratory analysis started, basic graphs made. More progress made on remaining games from round robin
</commit_message>
<xml_diff>
--- a/data/raw/pbr_roundrobin_6_1_2025.xlsx
+++ b/data/raw/pbr_roundrobin_6_1_2025.xlsx
@@ -8,17 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ryanhoffman/Desktop/development/ultimate-metrics/data/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F993EDCA-B160-2142-B569-2F201CC37C03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A961259-3E46-664B-8459-1ED0E1751074}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-380" yWindow="1000" windowWidth="34560" windowHeight="21580" xr2:uid="{38BF31FB-E6C4-0C4B-88A6-6097D42BA315}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" activeTab="1" xr2:uid="{38BF31FB-E6C4-0C4B-88A6-6097D42BA315}"/>
   </bookViews>
   <sheets>
     <sheet name="sunshine" sheetId="2" r:id="rId1"/>
+    <sheet name="mischief" sheetId="3" r:id="rId2"/>
+    <sheet name="bw" sheetId="5" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="gendercycle">sunshine!$AB$2:$AB$5</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -61,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="615" uniqueCount="271">
   <si>
     <t>tournament</t>
   </si>
@@ -441,9 +443,6 @@
     <t>huck to juleon down the line (unclear force)</t>
   </si>
   <si>
-    <t>the point only had one throw in it. Missing film</t>
-  </si>
-  <si>
     <t>three breaks into a breakside huck to score</t>
   </si>
   <si>
@@ -613,6 +612,270 @@
   </si>
   <si>
     <t>huck up the break side, margo capitlaized on slow defense</t>
+  </si>
+  <si>
+    <t>Point is missing film</t>
+  </si>
+  <si>
+    <t>mischief</t>
+  </si>
+  <si>
+    <t>g002</t>
+  </si>
+  <si>
+    <t>1-1</t>
+  </si>
+  <si>
+    <t>2-1</t>
+  </si>
+  <si>
+    <t>2-2</t>
+  </si>
+  <si>
+    <t>3-2</t>
+  </si>
+  <si>
+    <t>3-3</t>
+  </si>
+  <si>
+    <t>3-4</t>
+  </si>
+  <si>
+    <t>4-4</t>
+  </si>
+  <si>
+    <t>4-5</t>
+  </si>
+  <si>
+    <t>5-5</t>
+  </si>
+  <si>
+    <t>5-6</t>
+  </si>
+  <si>
+    <t>5-7</t>
+  </si>
+  <si>
+    <t>6-7</t>
+  </si>
+  <si>
+    <t>6-8</t>
+  </si>
+  <si>
+    <t>6-9</t>
+  </si>
+  <si>
+    <t>6-10</t>
+  </si>
+  <si>
+    <t>7-10</t>
+  </si>
+  <si>
+    <t>7-11</t>
+  </si>
+  <si>
+    <t>7-12</t>
+  </si>
+  <si>
+    <t>8-12</t>
+  </si>
+  <si>
+    <t>8-13</t>
+  </si>
+  <si>
+    <t>8-14</t>
+  </si>
+  <si>
+    <t>9-14</t>
+  </si>
+  <si>
+    <t>9-15</t>
+  </si>
+  <si>
+    <t>courtney,margo,malia,carol,eric,orion,sawyer</t>
+  </si>
+  <si>
+    <t>jesse,emma,visakha,emmet,carson,devin,jonah</t>
+  </si>
+  <si>
+    <t>aviva,jess,tuna,crawford,eric,yeagle,jack</t>
+  </si>
+  <si>
+    <t>molly,monica,ash,sara,selim,lincoln,seamus</t>
+  </si>
+  <si>
+    <t>courtney,cass,tuna,ruby,crawford,orion,juleon</t>
+  </si>
+  <si>
+    <t>jesse,emma,vail,carson,lincoln,seamus,princess</t>
+  </si>
+  <si>
+    <t>malia,margo,carol,emmet,tristan,yeagle,sawyer</t>
+  </si>
+  <si>
+    <t>aviva,courtney,jess,tuna,eric,orion,jack</t>
+  </si>
+  <si>
+    <t>molly,ash,visakha,vail,selim,devin,jonah</t>
+  </si>
+  <si>
+    <t>cass,margo,ruby,crawford,tristan,yeagle,juleon</t>
+  </si>
+  <si>
+    <t>jesse,monica,sara,carson,lincoln,seamus,princess</t>
+  </si>
+  <si>
+    <t>aviva,malia,jess,margo,crawford,eric,jack</t>
+  </si>
+  <si>
+    <t>courtney,molly,carol,ruby,emmet,orion,sawyer</t>
+  </si>
+  <si>
+    <t>cass,ash,emma,selim,lincoln,devin,jonah</t>
+  </si>
+  <si>
+    <t>jesse,sara,vail,tristan,selim,seamus,princess</t>
+  </si>
+  <si>
+    <t>aviva,malia,margo,tuna,crawford,orion,juleon</t>
+  </si>
+  <si>
+    <t>courtney,cass,jess,monica,eric,emmet,yeagle</t>
+  </si>
+  <si>
+    <t>molly,ash,visakha,carson,devin,sawyer,jonah</t>
+  </si>
+  <si>
+    <t>malia,carol,ruby,crawford,tristan,juleon,jack</t>
+  </si>
+  <si>
+    <t>jesse,molly,margo,emma,selim,orion,seamus</t>
+  </si>
+  <si>
+    <t>cass,monica,visakha,vail,carson,lincoln,princess</t>
+  </si>
+  <si>
+    <t>aviva,jess,tuna,eric,emmet,yeagle,jack</t>
+  </si>
+  <si>
+    <t>courtney,malia,sara,crawford,selim,sawyer,jonah</t>
+  </si>
+  <si>
+    <t>jesse,ash,emma,vail,tristan,devin,jonah</t>
+  </si>
+  <si>
+    <t>g003</t>
+  </si>
+  <si>
+    <t>bw</t>
+  </si>
+  <si>
+    <t>0-1</t>
+  </si>
+  <si>
+    <t>1-2</t>
+  </si>
+  <si>
+    <t>2-3</t>
+  </si>
+  <si>
+    <t>4-3</t>
+  </si>
+  <si>
+    <t>5-3</t>
+  </si>
+  <si>
+    <t>6-4</t>
+  </si>
+  <si>
+    <t>7-4</t>
+  </si>
+  <si>
+    <t>10-4</t>
+  </si>
+  <si>
+    <t>11-4</t>
+  </si>
+  <si>
+    <t>12-4</t>
+  </si>
+  <si>
+    <t>13-4</t>
+  </si>
+  <si>
+    <t>13-5</t>
+  </si>
+  <si>
+    <t>14-5</t>
+  </si>
+  <si>
+    <t>14-6</t>
+  </si>
+  <si>
+    <t>15-6</t>
+  </si>
+  <si>
+    <t>molly,monica,sara,carson,lincoln,seamus,sawyer</t>
+  </si>
+  <si>
+    <t>aviva,malia,jess,carol,emmet,orion,juleon</t>
+  </si>
+  <si>
+    <t>cass,ruby,ash,emma,tristan,selim,seamus</t>
+  </si>
+  <si>
+    <t>courtney,tuna,monica,eric,carson,yeagle,jack</t>
+  </si>
+  <si>
+    <t>jesse,visakha,vail,tristan,lincoln,devin,princess</t>
+  </si>
+  <si>
+    <t>aviva,malia,margo,carol,crawford,yeagle,jack</t>
+  </si>
+  <si>
+    <t>molly,ruby,sara,vail,emmet,juleon,seamus</t>
+  </si>
+  <si>
+    <t>jesse,ash,emma,selim,lincoln,devin,sawyer</t>
+  </si>
+  <si>
+    <t>cass,tuna,monica,eric,tristan,jack,princess</t>
+  </si>
+  <si>
+    <t>courtney,jess,margo,sara,emmet,carson,yeagle</t>
+  </si>
+  <si>
+    <t>aviva,malia,ruby,emma,crawford,orion,seamus</t>
+  </si>
+  <si>
+    <t>molly,carol,vail,eric,selim,juleon,sawyer</t>
+  </si>
+  <si>
+    <t>courtney,margo,tuna,crawford,tristan,yeagle,jack</t>
+  </si>
+  <si>
+    <t>cass,jesse,monica,ash,carson,lincoln,devin</t>
+  </si>
+  <si>
+    <t>molly,ruby,emma,sara,emmet,tristan,seamus</t>
+  </si>
+  <si>
+    <t>malia,jess,carol,eric,selim,jack,princess</t>
+  </si>
+  <si>
+    <t>cass,monica,vail,carson,selim,juleon,sawyer</t>
+  </si>
+  <si>
+    <t>courtney,margo,tuna,emma,lincoln,orion,devin</t>
+  </si>
+  <si>
+    <t>aviva,malia,ruby,sara,crawford,tristan,yeagle</t>
+  </si>
+  <si>
+    <t>jesse,molly,vail,emmet,jack,seamus,princess</t>
+  </si>
+  <si>
+    <t>cass,ash,emma,tristan,selim,lincoln,sawyer</t>
   </si>
 </sst>
 </file>
@@ -654,16 +917,45 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="5">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1003,8 +1295,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FACC20CB-3FA5-374C-9A70-9CEF466F05A9}">
   <dimension ref="A1:AB25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="157" zoomScaleNormal="157" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView zoomScale="157" zoomScaleNormal="157" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1053,37 +1345,37 @@
         <v>2</v>
       </c>
       <c r="J1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="L1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="M1" t="s">
         <v>33</v>
       </c>
       <c r="N1" t="s">
+        <v>172</v>
+      </c>
+      <c r="O1" t="s">
         <v>173</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>174</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>175</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>176</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>177</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>178</v>
-      </c>
-      <c r="T1" t="s">
-        <v>179</v>
       </c>
       <c r="U1" t="s">
         <v>3</v>
@@ -1092,10 +1384,10 @@
         <v>32</v>
       </c>
       <c r="W1" t="s">
+        <v>179</v>
+      </c>
+      <c r="X1" t="s">
         <v>180</v>
-      </c>
-      <c r="X1" t="s">
-        <v>181</v>
       </c>
       <c r="Y1" t="s">
         <v>1</v>
@@ -1176,7 +1468,7 @@
         <v>7</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>24</v>
@@ -1195,7 +1487,7 @@
         <v>6</v>
       </c>
       <c r="M3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="N3">
         <v>8</v>
@@ -1231,7 +1523,7 @@
         <v>23</v>
       </c>
       <c r="Y3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="AB3" t="s">
         <v>11</v>
@@ -1252,7 +1544,7 @@
         <v>7</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>28</v>
@@ -1417,7 +1709,7 @@
         <v>7</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>43</v>
@@ -1481,7 +1773,7 @@
         <v>7</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>58</v>
@@ -1500,7 +1792,7 @@
         <v>76</v>
       </c>
       <c r="M8" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="N8">
         <v>3</v>
@@ -1542,7 +1834,7 @@
         <v>7</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>46</v>
@@ -1609,7 +1901,7 @@
         <v>7</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>59</v>
@@ -1670,7 +1962,7 @@
         <v>7</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>49</v>
@@ -1740,7 +2032,7 @@
         <v>7</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>53</v>
@@ -1759,7 +2051,7 @@
         <v>6</v>
       </c>
       <c r="M12" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="N12">
         <v>5</v>
@@ -1813,7 +2105,7 @@
         <v>7</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>60</v>
@@ -1874,7 +2166,7 @@
         <v>7</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>61</v>
@@ -1926,7 +2218,7 @@
         <v>125</v>
       </c>
       <c r="Y14" t="s">
-        <v>126</v>
+        <v>183</v>
       </c>
     </row>
     <row r="15" spans="1:28" x14ac:dyDescent="0.2">
@@ -1944,7 +2236,7 @@
         <v>7</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>62</v>
@@ -1987,7 +2279,7 @@
         <v>7</v>
       </c>
       <c r="X15" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="16" spans="1:28" x14ac:dyDescent="0.2">
@@ -2005,7 +2297,7 @@
         <v>7</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>63</v>
@@ -2021,7 +2313,7 @@
         <v>5</v>
       </c>
       <c r="M16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="N16">
         <v>10</v>
@@ -2051,13 +2343,13 @@
         <v>21</v>
       </c>
       <c r="W16" t="s">
+        <v>128</v>
+      </c>
+      <c r="X16" t="s">
         <v>129</v>
       </c>
-      <c r="X16" t="s">
-        <v>130</v>
-      </c>
       <c r="Y16" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="17" spans="1:24" x14ac:dyDescent="0.2">
@@ -2075,7 +2367,7 @@
         <v>7</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>64</v>
@@ -2118,7 +2410,7 @@
         <v>7</v>
       </c>
       <c r="X17" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="18" spans="1:24" x14ac:dyDescent="0.2">
@@ -2136,7 +2428,7 @@
         <v>7</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>65</v>
@@ -2179,7 +2471,7 @@
         <v>7</v>
       </c>
       <c r="X18" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="19" spans="1:24" x14ac:dyDescent="0.2">
@@ -2197,7 +2489,7 @@
         <v>7</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>66</v>
@@ -2216,7 +2508,7 @@
         <v>74</v>
       </c>
       <c r="M19" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="N19">
         <v>1</v>
@@ -2240,7 +2532,7 @@
         <v>122</v>
       </c>
       <c r="U19" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="V19" t="s">
         <v>15</v>
@@ -2249,7 +2541,7 @@
         <v>22</v>
       </c>
       <c r="X19" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="20" spans="1:24" x14ac:dyDescent="0.2">
@@ -2267,7 +2559,7 @@
         <v>7</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>67</v>
@@ -2313,13 +2605,13 @@
         <v>36</v>
       </c>
       <c r="V20" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="W20" t="s">
         <v>30</v>
       </c>
       <c r="X20" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="21" spans="1:24" x14ac:dyDescent="0.2">
@@ -2337,7 +2629,7 @@
         <v>7</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>68</v>
@@ -2380,7 +2672,7 @@
         <v>7</v>
       </c>
       <c r="X21" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="22" spans="1:24" x14ac:dyDescent="0.2">
@@ -2398,7 +2690,7 @@
         <v>7</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>69</v>
@@ -2441,16 +2733,16 @@
         <v>122</v>
       </c>
       <c r="U22" t="s">
+        <v>160</v>
+      </c>
+      <c r="V22" t="s">
+        <v>159</v>
+      </c>
+      <c r="W22" t="s">
+        <v>128</v>
+      </c>
+      <c r="X22" t="s">
         <v>161</v>
-      </c>
-      <c r="V22" t="s">
-        <v>160</v>
-      </c>
-      <c r="W22" t="s">
-        <v>129</v>
-      </c>
-      <c r="X22" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="23" spans="1:24" x14ac:dyDescent="0.2">
@@ -2468,7 +2760,7 @@
         <v>7</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>70</v>
@@ -2511,7 +2803,7 @@
         <v>7</v>
       </c>
       <c r="X23" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="24" spans="1:24" x14ac:dyDescent="0.2">
@@ -2529,7 +2821,7 @@
         <v>7</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>71</v>
@@ -2569,16 +2861,16 @@
         <v>122</v>
       </c>
       <c r="U24" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="V24" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="W24" t="s">
         <v>80</v>
       </c>
       <c r="X24" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="25" spans="1:24" x14ac:dyDescent="0.2">
@@ -2596,7 +2888,7 @@
         <v>7</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>72</v>
@@ -2642,19 +2934,19 @@
         <v>37</v>
       </c>
       <c r="V25" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="W25" t="s">
         <v>17</v>
       </c>
       <c r="X25" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="A1:Y54">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="4" priority="1">
       <formula>ISEVEN(ROW())</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2664,4 +2956,1533 @@
     <ignoredError sqref="F2:F6" twoDigitTextYear="1"/>
   </ignoredErrors>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75D2B8A5-098E-5042-AE7E-61911D94C706}">
+  <dimension ref="A1:Y25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="6" max="6" width="10.83203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J1" t="s">
+        <v>171</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="L1" t="s">
+        <v>165</v>
+      </c>
+      <c r="M1" t="s">
+        <v>33</v>
+      </c>
+      <c r="N1" t="s">
+        <v>172</v>
+      </c>
+      <c r="O1" t="s">
+        <v>173</v>
+      </c>
+      <c r="P1" t="s">
+        <v>174</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>175</v>
+      </c>
+      <c r="R1" t="s">
+        <v>176</v>
+      </c>
+      <c r="S1" t="s">
+        <v>177</v>
+      </c>
+      <c r="T1" t="s">
+        <v>178</v>
+      </c>
+      <c r="U1" t="s">
+        <v>3</v>
+      </c>
+      <c r="V1" t="s">
+        <v>32</v>
+      </c>
+      <c r="W1" t="s">
+        <v>179</v>
+      </c>
+      <c r="X1" t="s">
+        <v>180</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>185</v>
+      </c>
+      <c r="B2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" t="s">
+        <v>184</v>
+      </c>
+      <c r="E2" s="4">
+        <v>0</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" t="s">
+        <v>56</v>
+      </c>
+      <c r="M2" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A3" t="str">
+        <f>$A$2</f>
+        <v>g002</v>
+      </c>
+      <c r="B3" t="s">
+        <v>96</v>
+      </c>
+      <c r="C3" t="str">
+        <f>$C$2</f>
+        <v>rr1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>184</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="G3" t="str" cm="1">
+        <f t="array" ref="G3">INDEX(gendercycle, MOD(MATCH($G$2, gendercycle, 0) - 1 + ROW() - 2, 4) + 1)</f>
+        <v>c1</v>
+      </c>
+      <c r="H3" t="s">
+        <v>57</v>
+      </c>
+      <c r="M3" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A4" t="str">
+        <f t="shared" ref="A4:A25" si="0">$A$2</f>
+        <v>g002</v>
+      </c>
+      <c r="B4" t="s">
+        <v>97</v>
+      </c>
+      <c r="C4" t="str">
+        <f t="shared" ref="C4:C25" si="1">$C$2</f>
+        <v>rr1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>184</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="G4" t="str" cm="1">
+        <f t="array" ref="G4">INDEX(gendercycle, MOD(MATCH($G$2, gendercycle, 0) - 1 + ROW() - 2, 4) + 1)</f>
+        <v>c2</v>
+      </c>
+      <c r="H4" t="s">
+        <v>56</v>
+      </c>
+      <c r="M4" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A5" t="str">
+        <f t="shared" si="0"/>
+        <v>g002</v>
+      </c>
+      <c r="B5" t="s">
+        <v>98</v>
+      </c>
+      <c r="C5" t="str">
+        <f t="shared" si="1"/>
+        <v>rr1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>184</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="G5" t="str" cm="1">
+        <f t="array" ref="G5">INDEX(gendercycle, MOD(MATCH($G$2, gendercycle, 0) - 1 + ROW() - 2, 4) + 1)</f>
+        <v>f1</v>
+      </c>
+      <c r="H5" t="s">
+        <v>57</v>
+      </c>
+      <c r="M5" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A6" t="str">
+        <f t="shared" si="0"/>
+        <v>g002</v>
+      </c>
+      <c r="B6" t="s">
+        <v>99</v>
+      </c>
+      <c r="C6" t="str">
+        <f t="shared" si="1"/>
+        <v>rr1</v>
+      </c>
+      <c r="D6" t="s">
+        <v>184</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="G6" t="str" cm="1">
+        <f t="array" ref="G6">INDEX(gendercycle, MOD(MATCH($G$2, gendercycle, 0) - 1 + ROW() - 2, 4) + 1)</f>
+        <v>f2</v>
+      </c>
+      <c r="H6" t="s">
+        <v>56</v>
+      </c>
+      <c r="M6" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A7" t="str">
+        <f t="shared" si="0"/>
+        <v>g002</v>
+      </c>
+      <c r="B7" t="s">
+        <v>100</v>
+      </c>
+      <c r="C7" t="str">
+        <f t="shared" si="1"/>
+        <v>rr1</v>
+      </c>
+      <c r="D7" t="s">
+        <v>184</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="G7" t="str" cm="1">
+        <f t="array" ref="G7">INDEX(gendercycle, MOD(MATCH($G$2, gendercycle, 0) - 1 + ROW() - 2, 4) + 1)</f>
+        <v>c1</v>
+      </c>
+      <c r="H7" t="s">
+        <v>57</v>
+      </c>
+      <c r="M7" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A8" t="str">
+        <f t="shared" si="0"/>
+        <v>g002</v>
+      </c>
+      <c r="B8" t="s">
+        <v>101</v>
+      </c>
+      <c r="C8" t="str">
+        <f t="shared" si="1"/>
+        <v>rr1</v>
+      </c>
+      <c r="D8" t="s">
+        <v>184</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="G8" t="str" cm="1">
+        <f t="array" ref="G8">INDEX(gendercycle, MOD(MATCH($G$2, gendercycle, 0) - 1 + ROW() - 2, 4) + 1)</f>
+        <v>c2</v>
+      </c>
+      <c r="H8" t="s">
+        <v>56</v>
+      </c>
+      <c r="M8" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A9" t="str">
+        <f t="shared" si="0"/>
+        <v>g002</v>
+      </c>
+      <c r="B9" t="s">
+        <v>102</v>
+      </c>
+      <c r="C9" t="str">
+        <f t="shared" si="1"/>
+        <v>rr1</v>
+      </c>
+      <c r="D9" t="s">
+        <v>184</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="G9" t="str" cm="1">
+        <f t="array" ref="G9">INDEX(gendercycle, MOD(MATCH($G$2, gendercycle, 0) - 1 + ROW() - 2, 4) + 1)</f>
+        <v>f1</v>
+      </c>
+      <c r="H9" t="s">
+        <v>56</v>
+      </c>
+      <c r="M9" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A10" t="str">
+        <f t="shared" si="0"/>
+        <v>g002</v>
+      </c>
+      <c r="B10" t="s">
+        <v>103</v>
+      </c>
+      <c r="C10" t="str">
+        <f t="shared" si="1"/>
+        <v>rr1</v>
+      </c>
+      <c r="D10" t="s">
+        <v>184</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="G10" t="str" cm="1">
+        <f t="array" ref="G10">INDEX(gendercycle, MOD(MATCH($G$2, gendercycle, 0) - 1 + ROW() - 2, 4) + 1)</f>
+        <v>f2</v>
+      </c>
+      <c r="H10" t="s">
+        <v>57</v>
+      </c>
+      <c r="M10" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="11" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A11" t="str">
+        <f t="shared" si="0"/>
+        <v>g002</v>
+      </c>
+      <c r="B11" t="s">
+        <v>104</v>
+      </c>
+      <c r="C11" t="str">
+        <f t="shared" si="1"/>
+        <v>rr1</v>
+      </c>
+      <c r="D11" t="s">
+        <v>184</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="G11" t="str" cm="1">
+        <f t="array" ref="G11">INDEX(gendercycle, MOD(MATCH($G$2, gendercycle, 0) - 1 + ROW() - 2, 4) + 1)</f>
+        <v>c1</v>
+      </c>
+      <c r="H11" t="s">
+        <v>56</v>
+      </c>
+      <c r="M11" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="12" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A12" t="str">
+        <f t="shared" si="0"/>
+        <v>g002</v>
+      </c>
+      <c r="B12" t="s">
+        <v>105</v>
+      </c>
+      <c r="C12" t="str">
+        <f t="shared" si="1"/>
+        <v>rr1</v>
+      </c>
+      <c r="D12" t="s">
+        <v>184</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="G12" t="str" cm="1">
+        <f t="array" ref="G12">INDEX(gendercycle, MOD(MATCH($G$2, gendercycle, 0) - 1 + ROW() - 2, 4) + 1)</f>
+        <v>c2</v>
+      </c>
+      <c r="H12" t="s">
+        <v>57</v>
+      </c>
+      <c r="M12" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="13" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A13" t="str">
+        <f t="shared" si="0"/>
+        <v>g002</v>
+      </c>
+      <c r="B13" t="s">
+        <v>106</v>
+      </c>
+      <c r="C13" t="str">
+        <f t="shared" si="1"/>
+        <v>rr1</v>
+      </c>
+      <c r="D13" t="s">
+        <v>184</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="G13" t="str" cm="1">
+        <f t="array" ref="G13">INDEX(gendercycle, MOD(MATCH($G$2, gendercycle, 0) - 1 + ROW() - 2, 4) + 1)</f>
+        <v>f1</v>
+      </c>
+      <c r="H13" t="s">
+        <v>56</v>
+      </c>
+      <c r="M13" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="14" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A14" t="str">
+        <f t="shared" si="0"/>
+        <v>g002</v>
+      </c>
+      <c r="B14" t="s">
+        <v>107</v>
+      </c>
+      <c r="C14" t="str">
+        <f t="shared" si="1"/>
+        <v>rr1</v>
+      </c>
+      <c r="D14" t="s">
+        <v>184</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="G14" t="str" cm="1">
+        <f t="array" ref="G14">INDEX(gendercycle, MOD(MATCH($G$2, gendercycle, 0) - 1 + ROW() - 2, 4) + 1)</f>
+        <v>f2</v>
+      </c>
+      <c r="H14" t="s">
+        <v>56</v>
+      </c>
+      <c r="M14" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="15" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A15" t="str">
+        <f t="shared" si="0"/>
+        <v>g002</v>
+      </c>
+      <c r="B15" t="s">
+        <v>108</v>
+      </c>
+      <c r="C15" t="str">
+        <f t="shared" si="1"/>
+        <v>rr1</v>
+      </c>
+      <c r="D15" t="s">
+        <v>184</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="G15" t="str" cm="1">
+        <f t="array" ref="G15">INDEX(gendercycle, MOD(MATCH($G$2, gendercycle, 0) - 1 + ROW() - 2, 4) + 1)</f>
+        <v>c1</v>
+      </c>
+      <c r="H15" t="s">
+        <v>57</v>
+      </c>
+      <c r="M15" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="16" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A16" t="str">
+        <f t="shared" si="0"/>
+        <v>g002</v>
+      </c>
+      <c r="B16" t="s">
+        <v>109</v>
+      </c>
+      <c r="C16" t="str">
+        <f t="shared" si="1"/>
+        <v>rr1</v>
+      </c>
+      <c r="D16" t="s">
+        <v>184</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="G16" t="str" cm="1">
+        <f t="array" ref="G16">INDEX(gendercycle, MOD(MATCH($G$2, gendercycle, 0) - 1 + ROW() - 2, 4) + 1)</f>
+        <v>c2</v>
+      </c>
+      <c r="H16" t="s">
+        <v>57</v>
+      </c>
+      <c r="M16" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A17" t="str">
+        <f t="shared" si="0"/>
+        <v>g002</v>
+      </c>
+      <c r="B17" t="s">
+        <v>110</v>
+      </c>
+      <c r="C17" t="str">
+        <f t="shared" si="1"/>
+        <v>rr1</v>
+      </c>
+      <c r="D17" t="s">
+        <v>184</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="G17" t="str" cm="1">
+        <f t="array" ref="G17">INDEX(gendercycle, MOD(MATCH($G$2, gendercycle, 0) - 1 + ROW() - 2, 4) + 1)</f>
+        <v>f1</v>
+      </c>
+      <c r="H17" t="s">
+        <v>56</v>
+      </c>
+      <c r="M17" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A18" t="str">
+        <f t="shared" si="0"/>
+        <v>g002</v>
+      </c>
+      <c r="B18" t="s">
+        <v>111</v>
+      </c>
+      <c r="C18" t="str">
+        <f t="shared" si="1"/>
+        <v>rr1</v>
+      </c>
+      <c r="D18" t="s">
+        <v>184</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="G18" t="str" cm="1">
+        <f t="array" ref="G18">INDEX(gendercycle, MOD(MATCH($G$2, gendercycle, 0) - 1 + ROW() - 2, 4) + 1)</f>
+        <v>f2</v>
+      </c>
+      <c r="H18" t="s">
+        <v>56</v>
+      </c>
+      <c r="M18" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A19" t="str">
+        <f t="shared" si="0"/>
+        <v>g002</v>
+      </c>
+      <c r="B19" t="s">
+        <v>112</v>
+      </c>
+      <c r="C19" t="str">
+        <f t="shared" si="1"/>
+        <v>rr1</v>
+      </c>
+      <c r="D19" t="s">
+        <v>184</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="G19" t="str" cm="1">
+        <f t="array" ref="G19">INDEX(gendercycle, MOD(MATCH($G$2, gendercycle, 0) - 1 + ROW() - 2, 4) + 1)</f>
+        <v>c1</v>
+      </c>
+      <c r="H19" t="s">
+        <v>57</v>
+      </c>
+      <c r="M19" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A20" t="str">
+        <f t="shared" si="0"/>
+        <v>g002</v>
+      </c>
+      <c r="B20" t="s">
+        <v>113</v>
+      </c>
+      <c r="C20" t="str">
+        <f t="shared" si="1"/>
+        <v>rr1</v>
+      </c>
+      <c r="D20" t="s">
+        <v>184</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="G20" t="str" cm="1">
+        <f t="array" ref="G20">INDEX(gendercycle, MOD(MATCH($G$2, gendercycle, 0) - 1 + ROW() - 2, 4) + 1)</f>
+        <v>c2</v>
+      </c>
+      <c r="H20" t="s">
+        <v>56</v>
+      </c>
+      <c r="M20" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A21" t="str">
+        <f t="shared" si="0"/>
+        <v>g002</v>
+      </c>
+      <c r="B21" t="s">
+        <v>114</v>
+      </c>
+      <c r="C21" t="str">
+        <f t="shared" si="1"/>
+        <v>rr1</v>
+      </c>
+      <c r="D21" t="s">
+        <v>184</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="G21" t="str" cm="1">
+        <f t="array" ref="G21">INDEX(gendercycle, MOD(MATCH($G$2, gendercycle, 0) - 1 + ROW() - 2, 4) + 1)</f>
+        <v>f1</v>
+      </c>
+      <c r="H21" t="s">
+        <v>56</v>
+      </c>
+      <c r="M21" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A22" t="str">
+        <f t="shared" si="0"/>
+        <v>g002</v>
+      </c>
+      <c r="B22" t="s">
+        <v>115</v>
+      </c>
+      <c r="C22" t="str">
+        <f t="shared" si="1"/>
+        <v>rr1</v>
+      </c>
+      <c r="D22" t="s">
+        <v>184</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="G22" t="str" cm="1">
+        <f t="array" ref="G22">INDEX(gendercycle, MOD(MATCH($G$2, gendercycle, 0) - 1 + ROW() - 2, 4) + 1)</f>
+        <v>f2</v>
+      </c>
+      <c r="H22" t="s">
+        <v>57</v>
+      </c>
+      <c r="M22" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A23" t="str">
+        <f t="shared" si="0"/>
+        <v>g002</v>
+      </c>
+      <c r="B23" t="s">
+        <v>116</v>
+      </c>
+      <c r="C23" t="str">
+        <f t="shared" si="1"/>
+        <v>rr1</v>
+      </c>
+      <c r="D23" t="s">
+        <v>184</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="G23" t="str" cm="1">
+        <f t="array" ref="G23">INDEX(gendercycle, MOD(MATCH($G$2, gendercycle, 0) - 1 + ROW() - 2, 4) + 1)</f>
+        <v>c1</v>
+      </c>
+      <c r="H23" t="s">
+        <v>56</v>
+      </c>
+      <c r="M23" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A24" t="str">
+        <f t="shared" si="0"/>
+        <v>g002</v>
+      </c>
+      <c r="B24" t="s">
+        <v>117</v>
+      </c>
+      <c r="C24" t="str">
+        <f t="shared" si="1"/>
+        <v>rr1</v>
+      </c>
+      <c r="D24" t="s">
+        <v>184</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="G24" t="str" cm="1">
+        <f t="array" ref="G24">INDEX(gendercycle, MOD(MATCH($G$2, gendercycle, 0) - 1 + ROW() - 2, 4) + 1)</f>
+        <v>c2</v>
+      </c>
+      <c r="H24" t="s">
+        <v>56</v>
+      </c>
+      <c r="M24" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A25" t="str">
+        <f t="shared" si="0"/>
+        <v>g002</v>
+      </c>
+      <c r="B25" t="s">
+        <v>118</v>
+      </c>
+      <c r="C25" t="str">
+        <f t="shared" si="1"/>
+        <v>rr1</v>
+      </c>
+      <c r="D25" t="s">
+        <v>184</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="G25" t="str" cm="1">
+        <f t="array" ref="G25">INDEX(gendercycle, MOD(MATCH($G$2, gendercycle, 0) - 1 + ROW() - 2, 4) + 1)</f>
+        <v>f1</v>
+      </c>
+      <c r="H25" t="s">
+        <v>57</v>
+      </c>
+      <c r="M25" t="s">
+        <v>232</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <conditionalFormatting sqref="A1:Y1">
+    <cfRule type="expression" dxfId="3" priority="2">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1:Y25">
+    <cfRule type="expression" dxfId="1" priority="1">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="F2" twoDigitTextYear="1"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9447876-9DC0-0C46-8C6A-6165F8BF6A0B}">
+  <dimension ref="A1:AB22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M23" sqref="M23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="6" max="6" width="10.83203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J1" t="s">
+        <v>171</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="L1" t="s">
+        <v>165</v>
+      </c>
+      <c r="M1" t="s">
+        <v>33</v>
+      </c>
+      <c r="N1" t="s">
+        <v>172</v>
+      </c>
+      <c r="O1" t="s">
+        <v>173</v>
+      </c>
+      <c r="P1" t="s">
+        <v>174</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>175</v>
+      </c>
+      <c r="R1" t="s">
+        <v>176</v>
+      </c>
+      <c r="S1" t="s">
+        <v>177</v>
+      </c>
+      <c r="T1" t="s">
+        <v>178</v>
+      </c>
+      <c r="U1" t="s">
+        <v>3</v>
+      </c>
+      <c r="V1" t="s">
+        <v>32</v>
+      </c>
+      <c r="W1" t="s">
+        <v>179</v>
+      </c>
+      <c r="X1" t="s">
+        <v>180</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>233</v>
+      </c>
+      <c r="B2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" t="s">
+        <v>234</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="G2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" t="s">
+        <v>57</v>
+      </c>
+      <c r="M2" t="s">
+        <v>250</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A3" t="str">
+        <f>$A$2</f>
+        <v>g003</v>
+      </c>
+      <c r="B3" t="s">
+        <v>96</v>
+      </c>
+      <c r="C3" t="str">
+        <f>$C$2</f>
+        <v>rr1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>234</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="G3" t="str" cm="1">
+        <f t="array" ref="G3">INDEX(gendercycle, MOD(MATCH($G$2, gendercycle, 0) - 1 + ROW() - 2, 4) + 1)</f>
+        <v>f1</v>
+      </c>
+      <c r="H3" t="s">
+        <v>56</v>
+      </c>
+      <c r="M3" t="s">
+        <v>251</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A4" t="str">
+        <f t="shared" ref="A4:A22" si="0">$A$2</f>
+        <v>g003</v>
+      </c>
+      <c r="B4" t="s">
+        <v>97</v>
+      </c>
+      <c r="C4" t="str">
+        <f t="shared" ref="C4:C22" si="1">$C$2</f>
+        <v>rr1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>234</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="G4" t="str" cm="1">
+        <f t="array" ref="G4">INDEX(gendercycle, MOD(MATCH($G$2, gendercycle, 0) - 1 + ROW() - 2, 4) + 1)</f>
+        <v>f2</v>
+      </c>
+      <c r="H4" t="s">
+        <v>57</v>
+      </c>
+      <c r="M4" t="s">
+        <v>252</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A5" t="str">
+        <f t="shared" si="0"/>
+        <v>g003</v>
+      </c>
+      <c r="B5" t="s">
+        <v>98</v>
+      </c>
+      <c r="C5" t="str">
+        <f t="shared" si="1"/>
+        <v>rr1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>234</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="G5" t="str" cm="1">
+        <f t="array" ref="G5">INDEX(gendercycle, MOD(MATCH($G$2, gendercycle, 0) - 1 + ROW() - 2, 4) + 1)</f>
+        <v>c1</v>
+      </c>
+      <c r="H5" t="s">
+        <v>56</v>
+      </c>
+      <c r="M5" t="s">
+        <v>253</v>
+      </c>
+      <c r="AB5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A6" t="str">
+        <f t="shared" si="0"/>
+        <v>g003</v>
+      </c>
+      <c r="B6" t="s">
+        <v>99</v>
+      </c>
+      <c r="C6" t="str">
+        <f t="shared" si="1"/>
+        <v>rr1</v>
+      </c>
+      <c r="D6" t="s">
+        <v>234</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="G6" t="str" cm="1">
+        <f t="array" ref="G6">INDEX(gendercycle, MOD(MATCH($G$2, gendercycle, 0) - 1 + ROW() - 2, 4) + 1)</f>
+        <v>c2</v>
+      </c>
+      <c r="H6" t="s">
+        <v>57</v>
+      </c>
+      <c r="M6" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="7" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A7" t="str">
+        <f t="shared" si="0"/>
+        <v>g003</v>
+      </c>
+      <c r="B7" t="s">
+        <v>100</v>
+      </c>
+      <c r="C7" t="str">
+        <f t="shared" si="1"/>
+        <v>rr1</v>
+      </c>
+      <c r="D7" t="s">
+        <v>234</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="G7" t="str" cm="1">
+        <f t="array" ref="G7">INDEX(gendercycle, MOD(MATCH($G$2, gendercycle, 0) - 1 + ROW() - 2, 4) + 1)</f>
+        <v>f1</v>
+      </c>
+      <c r="H7" t="s">
+        <v>56</v>
+      </c>
+      <c r="M7" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="8" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A8" t="str">
+        <f t="shared" si="0"/>
+        <v>g003</v>
+      </c>
+      <c r="B8" t="s">
+        <v>101</v>
+      </c>
+      <c r="C8" t="str">
+        <f t="shared" si="1"/>
+        <v>rr1</v>
+      </c>
+      <c r="D8" t="s">
+        <v>234</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="G8" t="str" cm="1">
+        <f t="array" ref="G8">INDEX(gendercycle, MOD(MATCH($G$2, gendercycle, 0) - 1 + ROW() - 2, 4) + 1)</f>
+        <v>f2</v>
+      </c>
+      <c r="H8" t="s">
+        <v>57</v>
+      </c>
+      <c r="M8" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="9" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A9" t="str">
+        <f t="shared" si="0"/>
+        <v>g003</v>
+      </c>
+      <c r="B9" t="s">
+        <v>102</v>
+      </c>
+      <c r="C9" t="str">
+        <f t="shared" si="1"/>
+        <v>rr1</v>
+      </c>
+      <c r="D9" t="s">
+        <v>234</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="G9" t="str" cm="1">
+        <f t="array" ref="G9">INDEX(gendercycle, MOD(MATCH($G$2, gendercycle, 0) - 1 + ROW() - 2, 4) + 1)</f>
+        <v>c1</v>
+      </c>
+      <c r="H9" t="s">
+        <v>57</v>
+      </c>
+      <c r="M9" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="10" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A10" t="str">
+        <f t="shared" si="0"/>
+        <v>g003</v>
+      </c>
+      <c r="B10" t="s">
+        <v>103</v>
+      </c>
+      <c r="C10" t="str">
+        <f t="shared" si="1"/>
+        <v>rr1</v>
+      </c>
+      <c r="D10" t="s">
+        <v>234</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="G10" t="str" cm="1">
+        <f t="array" ref="G10">INDEX(gendercycle, MOD(MATCH($G$2, gendercycle, 0) - 1 + ROW() - 2, 4) + 1)</f>
+        <v>c2</v>
+      </c>
+      <c r="H10" t="s">
+        <v>57</v>
+      </c>
+      <c r="M10" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="11" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A11" t="str">
+        <f t="shared" si="0"/>
+        <v>g003</v>
+      </c>
+      <c r="B11" t="s">
+        <v>104</v>
+      </c>
+      <c r="C11" t="str">
+        <f t="shared" si="1"/>
+        <v>rr1</v>
+      </c>
+      <c r="D11" t="s">
+        <v>234</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="G11" t="str" cm="1">
+        <f t="array" ref="G11">INDEX(gendercycle, MOD(MATCH($G$2, gendercycle, 0) - 1 + ROW() - 2, 4) + 1)</f>
+        <v>f1</v>
+      </c>
+      <c r="H11" t="s">
+        <v>57</v>
+      </c>
+      <c r="M11" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="12" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A12" t="str">
+        <f t="shared" si="0"/>
+        <v>g003</v>
+      </c>
+      <c r="B12" t="s">
+        <v>105</v>
+      </c>
+      <c r="C12" t="str">
+        <f t="shared" si="1"/>
+        <v>rr1</v>
+      </c>
+      <c r="D12" t="s">
+        <v>234</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="G12" t="str" cm="1">
+        <f t="array" ref="G12">INDEX(gendercycle, MOD(MATCH($G$2, gendercycle, 0) - 1 + ROW() - 2, 4) + 1)</f>
+        <v>f2</v>
+      </c>
+      <c r="H12" t="s">
+        <v>56</v>
+      </c>
+      <c r="M12" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="13" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A13" t="str">
+        <f t="shared" si="0"/>
+        <v>g003</v>
+      </c>
+      <c r="B13" t="s">
+        <v>106</v>
+      </c>
+      <c r="C13" t="str">
+        <f t="shared" si="1"/>
+        <v>rr1</v>
+      </c>
+      <c r="D13" t="s">
+        <v>234</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G13" t="str" cm="1">
+        <f t="array" ref="G13">INDEX(gendercycle, MOD(MATCH($G$2, gendercycle, 0) - 1 + ROW() - 2, 4) + 1)</f>
+        <v>c1</v>
+      </c>
+      <c r="H13" t="s">
+        <v>57</v>
+      </c>
+      <c r="M13" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="14" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A14" t="str">
+        <f t="shared" si="0"/>
+        <v>g003</v>
+      </c>
+      <c r="B14" t="s">
+        <v>107</v>
+      </c>
+      <c r="C14" t="str">
+        <f t="shared" si="1"/>
+        <v>rr1</v>
+      </c>
+      <c r="D14" t="s">
+        <v>234</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G14" t="str" cm="1">
+        <f t="array" ref="G14">INDEX(gendercycle, MOD(MATCH($G$2, gendercycle, 0) - 1 + ROW() - 2, 4) + 1)</f>
+        <v>c2</v>
+      </c>
+      <c r="H14" t="s">
+        <v>56</v>
+      </c>
+      <c r="M14" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="15" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A15" t="str">
+        <f t="shared" si="0"/>
+        <v>g003</v>
+      </c>
+      <c r="B15" t="s">
+        <v>108</v>
+      </c>
+      <c r="C15" t="str">
+        <f t="shared" si="1"/>
+        <v>rr1</v>
+      </c>
+      <c r="D15" t="s">
+        <v>234</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="G15" t="str" cm="1">
+        <f t="array" ref="G15">INDEX(gendercycle, MOD(MATCH($G$2, gendercycle, 0) - 1 + ROW() - 2, 4) + 1)</f>
+        <v>f1</v>
+      </c>
+      <c r="H15" t="s">
+        <v>57</v>
+      </c>
+      <c r="M15" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="16" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A16" t="str">
+        <f t="shared" si="0"/>
+        <v>g003</v>
+      </c>
+      <c r="B16" t="s">
+        <v>109</v>
+      </c>
+      <c r="C16" t="str">
+        <f t="shared" si="1"/>
+        <v>rr1</v>
+      </c>
+      <c r="D16" t="s">
+        <v>234</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="G16" t="str" cm="1">
+        <f t="array" ref="G16">INDEX(gendercycle, MOD(MATCH($G$2, gendercycle, 0) - 1 + ROW() - 2, 4) + 1)</f>
+        <v>f2</v>
+      </c>
+      <c r="H16" t="s">
+        <v>57</v>
+      </c>
+      <c r="M16" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A17" t="str">
+        <f t="shared" si="0"/>
+        <v>g003</v>
+      </c>
+      <c r="B17" t="s">
+        <v>110</v>
+      </c>
+      <c r="C17" t="str">
+        <f t="shared" si="1"/>
+        <v>rr1</v>
+      </c>
+      <c r="D17" t="s">
+        <v>234</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="G17" t="str" cm="1">
+        <f t="array" ref="G17">INDEX(gendercycle, MOD(MATCH($G$2, gendercycle, 0) - 1 + ROW() - 2, 4) + 1)</f>
+        <v>c1</v>
+      </c>
+      <c r="H17" t="s">
+        <v>57</v>
+      </c>
+      <c r="M17" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A18" t="str">
+        <f t="shared" si="0"/>
+        <v>g003</v>
+      </c>
+      <c r="B18" t="s">
+        <v>111</v>
+      </c>
+      <c r="C18" t="str">
+        <f t="shared" si="1"/>
+        <v>rr1</v>
+      </c>
+      <c r="D18" t="s">
+        <v>234</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="G18" t="str" cm="1">
+        <f t="array" ref="G18">INDEX(gendercycle, MOD(MATCH($G$2, gendercycle, 0) - 1 + ROW() - 2, 4) + 1)</f>
+        <v>c2</v>
+      </c>
+      <c r="H18" t="s">
+        <v>57</v>
+      </c>
+      <c r="M18" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A19" t="str">
+        <f t="shared" si="0"/>
+        <v>g003</v>
+      </c>
+      <c r="B19" t="s">
+        <v>112</v>
+      </c>
+      <c r="C19" t="str">
+        <f t="shared" si="1"/>
+        <v>rr1</v>
+      </c>
+      <c r="D19" t="s">
+        <v>234</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="G19" t="str" cm="1">
+        <f t="array" ref="G19">INDEX(gendercycle, MOD(MATCH($G$2, gendercycle, 0) - 1 + ROW() - 2, 4) + 1)</f>
+        <v>f1</v>
+      </c>
+      <c r="H19" t="s">
+        <v>57</v>
+      </c>
+      <c r="M19" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A20" t="str">
+        <f t="shared" si="0"/>
+        <v>g003</v>
+      </c>
+      <c r="B20" t="s">
+        <v>113</v>
+      </c>
+      <c r="C20" t="str">
+        <f t="shared" si="1"/>
+        <v>rr1</v>
+      </c>
+      <c r="D20" t="s">
+        <v>234</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="G20" t="str" cm="1">
+        <f t="array" ref="G20">INDEX(gendercycle, MOD(MATCH($G$2, gendercycle, 0) - 1 + ROW() - 2, 4) + 1)</f>
+        <v>f2</v>
+      </c>
+      <c r="H20" t="s">
+        <v>56</v>
+      </c>
+      <c r="M20" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A21" t="str">
+        <f t="shared" si="0"/>
+        <v>g003</v>
+      </c>
+      <c r="B21" t="s">
+        <v>114</v>
+      </c>
+      <c r="C21" t="str">
+        <f t="shared" si="1"/>
+        <v>rr1</v>
+      </c>
+      <c r="D21" t="s">
+        <v>234</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="G21" t="str" cm="1">
+        <f t="array" ref="G21">INDEX(gendercycle, MOD(MATCH($G$2, gendercycle, 0) - 1 + ROW() - 2, 4) + 1)</f>
+        <v>c1</v>
+      </c>
+      <c r="H21" t="s">
+        <v>57</v>
+      </c>
+      <c r="M21" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A22" t="str">
+        <f t="shared" si="0"/>
+        <v>g003</v>
+      </c>
+      <c r="B22" t="s">
+        <v>115</v>
+      </c>
+      <c r="C22" t="str">
+        <f t="shared" si="1"/>
+        <v>rr1</v>
+      </c>
+      <c r="D22" t="s">
+        <v>234</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="G22" t="str" cm="1">
+        <f t="array" ref="G22">INDEX(gendercycle, MOD(MATCH($G$2, gendercycle, 0) - 1 + ROW() - 2, 4) + 1)</f>
+        <v>c2</v>
+      </c>
+      <c r="H22" t="s">
+        <v>56</v>
+      </c>
+      <c r="M22" t="s">
+        <v>270</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <conditionalFormatting sqref="A1:Y1">
+    <cfRule type="expression" dxfId="2" priority="2">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1:Y22">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>